<commit_message>
added equally weighted index
</commit_message>
<xml_diff>
--- a/Bollinger Bands Percentage.xlsx
+++ b/Bollinger Bands Percentage.xlsx
@@ -699,7 +699,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>-0.3176647585607476</v>
+        <v>-0.3176647585647625</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -710,7 +710,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>0.3094398213941567</v>
+        <v>0.3094398213942281</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -754,7 +754,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>0.9236265045972335</v>
+        <v>0.9236265045971936</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -765,7 +765,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>0.8767038824946926</v>
+        <v>0.8767038824946594</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -787,7 +787,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>0.7069083102788841</v>
+        <v>0.7069083102789145</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -798,7 +798,7 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>0.3210689215524677</v>
+        <v>0.3210689215529541</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -809,7 +809,7 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>0.9609339667505088</v>
+        <v>0.9609339667505202</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -831,7 +831,7 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>0.02064381400242256</v>
+        <v>0.02064381400224419</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -842,7 +842,7 @@
         <v>15</v>
       </c>
       <c r="C15">
-        <v>0.7481455138884409</v>
+        <v>0.7481455138883472</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -864,7 +864,7 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>1.045810780092423</v>
+        <v>1.045810780092351</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -875,7 +875,7 @@
         <v>18</v>
       </c>
       <c r="C18">
-        <v>1.083111064996225</v>
+        <v>1.08311106499626</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -886,7 +886,7 @@
         <v>19</v>
       </c>
       <c r="C19">
-        <v>0.3903162240761673</v>
+        <v>0.3903162240760032</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -897,7 +897,7 @@
         <v>20</v>
       </c>
       <c r="C20">
-        <v>0.4977147225944855</v>
+        <v>0.4977147225944863</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -908,7 +908,7 @@
         <v>21</v>
       </c>
       <c r="C21">
-        <v>0.8890511481829456</v>
+        <v>0.8890511481831271</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -919,7 +919,7 @@
         <v>22</v>
       </c>
       <c r="C22">
-        <v>0.9748661541227579</v>
+        <v>0.9748661541227296</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -930,7 +930,7 @@
         <v>23</v>
       </c>
       <c r="C23">
-        <v>0.7370218510105546</v>
+        <v>0.737021851010732</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -941,7 +941,7 @@
         <v>24</v>
       </c>
       <c r="C24">
-        <v>0.8478380122838366</v>
+        <v>0.8478380122837508</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -952,7 +952,7 @@
         <v>25</v>
       </c>
       <c r="C25">
-        <v>0.6202530485541545</v>
+        <v>0.6202530485535319</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -963,7 +963,7 @@
         <v>26</v>
       </c>
       <c r="C26">
-        <v>0.57185432122199</v>
+        <v>0.5718543212220566</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -974,7 +974,7 @@
         <v>27</v>
       </c>
       <c r="C27">
-        <v>0.9028796407414013</v>
+        <v>0.9028796407415371</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -985,7 +985,7 @@
         <v>28</v>
       </c>
       <c r="C28">
-        <v>0.4726551469653546</v>
+        <v>0.4726551469653568</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -996,7 +996,7 @@
         <v>29</v>
       </c>
       <c r="C29">
-        <v>0.4904203859209934</v>
+        <v>0.4904203859209667</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1007,7 +1007,7 @@
         <v>30</v>
       </c>
       <c r="C30">
-        <v>0.7533274076158747</v>
+        <v>0.7533274076151074</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1029,7 +1029,7 @@
         <v>32</v>
       </c>
       <c r="C32">
-        <v>0.8340525522406078</v>
+        <v>0.8340525522417556</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1040,7 +1040,7 @@
         <v>33</v>
       </c>
       <c r="C33">
-        <v>0.8340205357737929</v>
+        <v>0.8340205357735855</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1062,7 +1062,7 @@
         <v>35</v>
       </c>
       <c r="C35">
-        <v>0.6916058095660105</v>
+        <v>0.6916058095660116</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1073,7 +1073,7 @@
         <v>36</v>
       </c>
       <c r="C36">
-        <v>1.181096872959175</v>
+        <v>1.181096872959556</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1095,7 +1095,7 @@
         <v>38</v>
       </c>
       <c r="C38">
-        <v>0.8444820956380357</v>
+        <v>0.8444820956380091</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1117,7 +1117,7 @@
         <v>40</v>
       </c>
       <c r="C40">
-        <v>0.801539952255407</v>
+        <v>0.8015399522547344</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1128,7 +1128,7 @@
         <v>41</v>
       </c>
       <c r="C41">
-        <v>0.7506832294968839</v>
+        <v>0.7506832294967422</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1161,7 +1161,7 @@
         <v>44</v>
       </c>
       <c r="C44">
-        <v>1.216358599342322</v>
+        <v>1.216358599351481</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1172,7 +1172,7 @@
         <v>45</v>
       </c>
       <c r="C45">
-        <v>0.714068242892715</v>
+        <v>0.7140682428927331</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1183,7 +1183,7 @@
         <v>46</v>
       </c>
       <c r="C46">
-        <v>0.4592596854492532</v>
+        <v>0.4592596854492579</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1194,7 +1194,7 @@
         <v>47</v>
       </c>
       <c r="C47">
-        <v>0.5767491251222194</v>
+        <v>0.5767491251222298</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1205,7 +1205,7 @@
         <v>48</v>
       </c>
       <c r="C48">
-        <v>0.6833990034766164</v>
+        <v>0.6833990034766156</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1216,7 +1216,7 @@
         <v>49</v>
       </c>
       <c r="C49">
-        <v>1.029177729851284</v>
+        <v>1.029177729842099</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1227,7 +1227,7 @@
         <v>50</v>
       </c>
       <c r="C50">
-        <v>0.9205430760646812</v>
+        <v>0.9205430760646744</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1238,7 +1238,7 @@
         <v>51</v>
       </c>
       <c r="C51">
-        <v>0.8045691575497775</v>
+        <v>0.8045691575498112</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1260,7 +1260,7 @@
         <v>53</v>
       </c>
       <c r="C53">
-        <v>0.716595429884812</v>
+        <v>0.7165954298848143</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1271,7 +1271,7 @@
         <v>54</v>
       </c>
       <c r="C54">
-        <v>0.9691422457287541</v>
+        <v>0.9691422457433871</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1282,7 +1282,7 @@
         <v>55</v>
       </c>
       <c r="C55">
-        <v>0.7335244770579312</v>
+        <v>0.7335244770571361</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1293,7 +1293,7 @@
         <v>56</v>
       </c>
       <c r="C56">
-        <v>0.8545566134477852</v>
+        <v>0.8545566134485209</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1304,7 +1304,7 @@
         <v>57</v>
       </c>
       <c r="C57">
-        <v>0.5601867327867749</v>
+        <v>0.5601867327865649</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1315,7 +1315,7 @@
         <v>58</v>
       </c>
       <c r="C58">
-        <v>0.6843835186671483</v>
+        <v>0.6843835186671461</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1326,7 +1326,7 @@
         <v>59</v>
       </c>
       <c r="C59">
-        <v>1.036983495045283</v>
+        <v>1.036983495044219</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1337,7 +1337,7 @@
         <v>60</v>
       </c>
       <c r="C60">
-        <v>0.1354947743537337</v>
+        <v>0.1354947743537726</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1348,7 +1348,7 @@
         <v>61</v>
       </c>
       <c r="C61">
-        <v>0.3011533088848686</v>
+        <v>0.3011533088853706</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1359,7 +1359,7 @@
         <v>62</v>
       </c>
       <c r="C62">
-        <v>1.04371905131094</v>
+        <v>1.043719051308636</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1370,7 +1370,7 @@
         <v>63</v>
       </c>
       <c r="C63">
-        <v>0.9661156288430774</v>
+        <v>0.9661156288430933</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1381,7 +1381,7 @@
         <v>64</v>
       </c>
       <c r="C64">
-        <v>0.8430641204365136</v>
+        <v>0.8430641204364642</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1392,7 +1392,7 @@
         <v>65</v>
       </c>
       <c r="C65">
-        <v>0.6440115385921485</v>
+        <v>0.6440115385921442</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1403,7 +1403,7 @@
         <v>66</v>
       </c>
       <c r="C66">
-        <v>0.6598701140002583</v>
+        <v>0.6598701140002113</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -1414,7 +1414,7 @@
         <v>67</v>
       </c>
       <c r="C67">
-        <v>0.2073964725511491</v>
+        <v>0.2073964725473312</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1425,7 +1425,7 @@
         <v>68</v>
       </c>
       <c r="C68">
-        <v>0.5991317518670095</v>
+        <v>0.5991317518666264</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1436,7 +1436,7 @@
         <v>69</v>
       </c>
       <c r="C69">
-        <v>0.7042036638541983</v>
+        <v>0.7042036638536909</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1447,7 +1447,7 @@
         <v>70</v>
       </c>
       <c r="C70">
-        <v>0.6058434229832751</v>
+        <v>0.6058434229820716</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1458,7 +1458,7 @@
         <v>71</v>
       </c>
       <c r="C71">
-        <v>0.5745617658645278</v>
+        <v>0.5745617658642547</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1480,7 +1480,7 @@
         <v>73</v>
       </c>
       <c r="C73">
-        <v>0.8080485057828428</v>
+        <v>0.8080485057832661</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1491,7 +1491,7 @@
         <v>74</v>
       </c>
       <c r="C74">
-        <v>0.623914785796597</v>
+        <v>0.6239147857966959</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1502,7 +1502,7 @@
         <v>75</v>
       </c>
       <c r="C75">
-        <v>0.8442381207047266</v>
+        <v>0.8442381207047222</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1513,7 +1513,7 @@
         <v>76</v>
       </c>
       <c r="C76">
-        <v>0.9044696975420636</v>
+        <v>0.9044696975413156</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1524,7 +1524,7 @@
         <v>77</v>
       </c>
       <c r="C77">
-        <v>0.9824439390698835</v>
+        <v>0.9824439390698843</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1535,7 +1535,7 @@
         <v>78</v>
       </c>
       <c r="C78">
-        <v>0.8784573852696411</v>
+        <v>0.8784573852698109</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1557,7 +1557,7 @@
         <v>80</v>
       </c>
       <c r="C80">
-        <v>0.75751496495335</v>
+        <v>0.7575149649532484</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1568,7 +1568,7 @@
         <v>81</v>
       </c>
       <c r="C81">
-        <v>0.7349968280853231</v>
+        <v>0.7349968280853215</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1579,7 +1579,7 @@
         <v>82</v>
       </c>
       <c r="C82">
-        <v>0.5880029915698713</v>
+        <v>0.5880029915698733</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1590,7 +1590,7 @@
         <v>83</v>
       </c>
       <c r="C83">
-        <v>0.8892010870645163</v>
+        <v>0.8892010870641628</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1601,7 +1601,7 @@
         <v>84</v>
       </c>
       <c r="C84">
-        <v>0.5895580141487403</v>
+        <v>0.5895580141501728</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1612,7 +1612,7 @@
         <v>85</v>
       </c>
       <c r="C85">
-        <v>0.4910632923463819</v>
+        <v>0.4910632923463937</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1623,7 +1623,7 @@
         <v>86</v>
       </c>
       <c r="C86">
-        <v>0.8582681152662818</v>
+        <v>0.8582681152673486</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1634,7 +1634,7 @@
         <v>87</v>
       </c>
       <c r="C87">
-        <v>0.8449036201527466</v>
+        <v>0.8449036201527901</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1645,7 +1645,7 @@
         <v>88</v>
       </c>
       <c r="C88">
-        <v>0.7315485668312998</v>
+        <v>0.7315485668301482</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -1667,7 +1667,7 @@
         <v>90</v>
       </c>
       <c r="C90">
-        <v>0.3726786510688046</v>
+        <v>0.3726786510687627</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -1678,7 +1678,7 @@
         <v>91</v>
       </c>
       <c r="C91">
-        <v>0.7037122082070023</v>
+        <v>0.7037122082075636</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1689,7 +1689,7 @@
         <v>92</v>
       </c>
       <c r="C92">
-        <v>0.5667250669014953</v>
+        <v>0.5667250669016035</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1700,7 +1700,7 @@
         <v>93</v>
       </c>
       <c r="C93">
-        <v>0.8718533751442202</v>
+        <v>0.8718533751355505</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1711,7 +1711,7 @@
         <v>94</v>
       </c>
       <c r="C94">
-        <v>0.4230233325475747</v>
+        <v>0.4230233325483378</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1733,7 +1733,7 @@
         <v>96</v>
       </c>
       <c r="C96">
-        <v>0.6496896127629439</v>
+        <v>0.6496896127626216</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1744,7 +1744,7 @@
         <v>97</v>
       </c>
       <c r="C97">
-        <v>0.5603252987501089</v>
+        <v>0.5603252987501931</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1755,7 +1755,7 @@
         <v>98</v>
       </c>
       <c r="C98">
-        <v>1.124640090815902</v>
+        <v>1.124640090815987</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1766,7 +1766,7 @@
         <v>99</v>
       </c>
       <c r="C99">
-        <v>0.5513359614544515</v>
+        <v>0.5513359614547764</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1777,7 +1777,7 @@
         <v>100</v>
       </c>
       <c r="C100">
-        <v>0.5843299138663438</v>
+        <v>0.5843299138664421</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1788,7 +1788,7 @@
         <v>101</v>
       </c>
       <c r="C101">
-        <v>1.202133176770904</v>
+        <v>1.202133176768726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>